<commit_message>
updated taxonomy for watchlist
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_citsci_ms/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9FBABD-D6F5-FF44-8153-9E10E9342634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E8A73C-F171-1A47-BA60-B11D61EAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="178">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Actaea rubra</t>
   </si>
   <si>
-    <t>Agalinis paupercula</t>
-  </si>
-  <si>
     <t>Amphicarpaea bracteata</t>
   </si>
   <si>
-    <t>Andropogon gerardii</t>
-  </si>
-  <si>
     <t>Antennaria neglecta</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Atriplex glabriuscula</t>
   </si>
   <si>
-    <t>Atriplex subspicata</t>
-  </si>
-  <si>
     <t>Bartonia paniculata</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>Carex ormostachya</t>
   </si>
   <si>
-    <t>Carex weigandii</t>
-  </si>
-  <si>
     <t>Centaurea nigrescens</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>Cystopteris fragilis</t>
   </si>
   <si>
-    <t>Dasiphora floribunda</t>
-  </si>
-  <si>
     <t>Diphasiastrum digitatum</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>Hypericum prolificum</t>
   </si>
   <si>
-    <t>Hypopitys monotropa</t>
-  </si>
-  <si>
     <t>Impatiens glandulifera</t>
   </si>
   <si>
@@ -223,9 +205,6 @@
     <t>Mertensia maritima</t>
   </si>
   <si>
-    <t>Mertensis maritima</t>
-  </si>
-  <si>
     <t>Mollugo verticillata</t>
   </si>
   <si>
@@ -301,9 +280,6 @@
     <t>Suaeda calceoliformis</t>
   </si>
   <si>
-    <t>Swida rugosa</t>
-  </si>
-  <si>
     <t>Symplocarpus foetidus</t>
   </si>
   <si>
@@ -454,9 +430,6 @@
     <t>Cardamine impatiens</t>
   </si>
   <si>
-    <t>Celastrus orbiculata</t>
-  </si>
-  <si>
     <t>Centaurea stoebe</t>
   </si>
   <si>
@@ -469,9 +442,6 @@
     <t>Euonymus spp.</t>
   </si>
   <si>
-    <t>Fallopia japonica</t>
-  </si>
-  <si>
     <t>Heracleum mantegazzianum</t>
   </si>
   <si>
@@ -499,12 +469,6 @@
     <t>Solanum dulcamara</t>
   </si>
   <si>
-    <t>Verbascum thapsis</t>
-  </si>
-  <si>
-    <t>Berberis spp.</t>
-  </si>
-  <si>
     <t>Frangula alnus</t>
   </si>
   <si>
@@ -572,6 +536,39 @@
   </si>
   <si>
     <t>Bombus terricola</t>
+  </si>
+  <si>
+    <t>Agalinis purpurea</t>
+  </si>
+  <si>
+    <t>Andropogon gerardi</t>
+  </si>
+  <si>
+    <t>Celastrus orbiculatus</t>
+  </si>
+  <si>
+    <t>Reynoutria japonica</t>
+  </si>
+  <si>
+    <t>Verbascum thapsus</t>
+  </si>
+  <si>
+    <t>Atriplex dioica</t>
+  </si>
+  <si>
+    <t>Carex wiegandii</t>
+  </si>
+  <si>
+    <t>Dasiphora fruticosa</t>
+  </si>
+  <si>
+    <t>Monotropa hypopitys</t>
+  </si>
+  <si>
+    <t>Cornus rugosa</t>
+  </si>
+  <si>
+    <t>Berberis thunbergii</t>
   </si>
 </sst>
 </file>
@@ -923,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="N166" sqref="N166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,13 +934,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -951,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -962,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,1858 +970,1825 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C78" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C85" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C89" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C92" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C97" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B100" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B101" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C103" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B106" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C106" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C109" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C113" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C114" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C115" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C116" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C117" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C118" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C119" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="B120" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C120" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B121" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C121" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B122" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C122" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="B123" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C123" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B124" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C124" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C125" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C126" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B127" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C127" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B128" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C128" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C129" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C130" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C131" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C133" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C134" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C135" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C136" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C137" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B138" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C138" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C139" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C140" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C141" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B142" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C142" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C143" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B144" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C146" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C147" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>140</v>
+      </c>
+      <c r="B148" t="s">
         <v>147</v>
       </c>
-      <c r="B148" t="s">
-        <v>159</v>
-      </c>
       <c r="C148" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="B149" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C150" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B151" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C151" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C152" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C153" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="B154" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C154" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C155" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" t="s">
         <v>153</v>
       </c>
-      <c r="B156" t="s">
-        <v>159</v>
-      </c>
       <c r="C156" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="B157" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C157" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C158" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C159" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C160" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C161" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B162" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C162" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B163" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C163" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B164" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C164" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C165" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C166" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B167" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C167" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C168" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B169" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C169" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>174</v>
-      </c>
-      <c r="B170" t="s">
-        <v>165</v>
-      </c>
-      <c r="C170" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>177</v>
-      </c>
-      <c r="B171" t="s">
-        <v>176</v>
-      </c>
-      <c r="C171" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>178</v>
-      </c>
-      <c r="B172" t="s">
-        <v>176</v>
-      </c>
-      <c r="C172" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jesse's updates to watchlist
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_citsci_ms/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E8A73C-F171-1A47-BA60-B11D61EAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE20827-CF59-F94C-B1B5-0A9AF04CFA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24400" windowHeight="13880" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="189">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -361,9 +361,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Cynanchum louiseae</t>
-  </si>
-  <si>
     <t>Dioscorea polystachya</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>Elaeagnus umbellata</t>
   </si>
   <si>
-    <t>Euonymus spp.</t>
-  </si>
-  <si>
     <t>Heracleum mantegazzianum</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>Lonicera japonica</t>
   </si>
   <si>
-    <t>Lonicera spp.</t>
-  </si>
-  <si>
     <t>Lupinus polyphyllus</t>
   </si>
   <si>
@@ -569,16 +560,72 @@
   </si>
   <si>
     <t>Berberis thunbergii</t>
+  </si>
+  <si>
+    <t>Berberis vulgaris</t>
+  </si>
+  <si>
+    <t>Euonymus alatus</t>
+  </si>
+  <si>
+    <t>Lonicera maackii</t>
+  </si>
+  <si>
+    <t>Lonicera periclymenum</t>
+  </si>
+  <si>
+    <t>Lonicera tatarica</t>
+  </si>
+  <si>
+    <t>Adelges piceae</t>
+  </si>
+  <si>
+    <t>Amynthas agrestis</t>
+  </si>
+  <si>
+    <t>Amynthas corticis</t>
+  </si>
+  <si>
+    <t>Amynthas tokioensis</t>
+  </si>
+  <si>
+    <t>Amynthas sexpectatus</t>
+  </si>
+  <si>
+    <t>Amynthas diffringens</t>
+  </si>
+  <si>
+    <t>Amynthas gracilis</t>
+  </si>
+  <si>
+    <t>Vincetoxicum nigrum</t>
+  </si>
+  <si>
+    <t>Vincetoxicum rossicum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -601,13 +648,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -621,6 +673,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,13 +976,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
@@ -940,1203 +996,1203 @@
         <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
         <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
         <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
         <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
         <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
         <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
         <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
         <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
         <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
         <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
         <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
         <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="B46" t="s">
         <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
         <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
         <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
         <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
         <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
         <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
         <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
         <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
         <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
         <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
         <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
         <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
         <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
         <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="B76" t="s">
         <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
         <v>103</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
         <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
         <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
         <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B86" t="s">
         <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
         <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B88" t="s">
         <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B89" t="s">
         <v>103</v>
       </c>
       <c r="C89" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
         <v>103</v>
       </c>
       <c r="C92" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C93" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C95" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" t="s">
-        <v>103</v>
-      </c>
-      <c r="C96" t="s">
-        <v>149</v>
+      <c r="A96" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B97" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C97" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C98" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C100" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C101" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C102" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C103" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>94</v>
+      <c r="A104" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="B106" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C106" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C107" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="B109" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C109" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C110" t="s">
         <v>107</v>
@@ -2144,10 +2200,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C111" t="s">
         <v>107</v>
@@ -2155,10 +2211,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C112" t="s">
         <v>107</v>
@@ -2166,10 +2222,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C113" t="s">
         <v>107</v>
@@ -2177,10 +2233,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C114" t="s">
         <v>107</v>
@@ -2188,10 +2244,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C115" t="s">
         <v>107</v>
@@ -2199,10 +2255,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
@@ -2210,21 +2266,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C117" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
@@ -2232,109 +2288,109 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B119" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C119" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="B120" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C120" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C121" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C122" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C123" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B124" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C124" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="B125" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C125" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B126" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C126" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C127" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B128" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C128" t="s">
         <v>105</v>
@@ -2342,21 +2398,21 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C129" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="B130" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C130" t="s">
         <v>105</v>
@@ -2364,10 +2420,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C131" t="s">
         <v>105</v>
@@ -2375,10 +2431,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C132" t="s">
         <v>105</v>
@@ -2386,10 +2442,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C133" t="s">
         <v>105</v>
@@ -2397,10 +2453,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C134" t="s">
         <v>105</v>
@@ -2408,10 +2464,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C135" t="s">
         <v>105</v>
@@ -2419,10 +2475,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="B136" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C136" t="s">
         <v>105</v>
@@ -2430,10 +2486,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>146</v>
+        <v>38</v>
       </c>
       <c r="B137" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C137" t="s">
         <v>105</v>
@@ -2441,10 +2497,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>145</v>
-      </c>
-      <c r="B138" t="s">
-        <v>147</v>
+        <v>44</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C138" t="s">
         <v>105</v>
@@ -2452,10 +2508,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="B139" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C139" t="s">
         <v>105</v>
@@ -2463,10 +2519,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="B140" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C140" t="s">
         <v>105</v>
@@ -2474,10 +2530,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C141" t="s">
         <v>105</v>
@@ -2485,10 +2541,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="B142" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C142" t="s">
         <v>105</v>
@@ -2496,10 +2552,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B143" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C143" t="s">
         <v>105</v>
@@ -2507,10 +2563,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="B144" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C144" t="s">
         <v>105</v>
@@ -2518,10 +2574,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C145" t="s">
         <v>105</v>
@@ -2529,10 +2585,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B146" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C146" t="s">
         <v>105</v>
@@ -2540,10 +2596,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C147" t="s">
         <v>105</v>
@@ -2551,10 +2607,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B148" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C148" t="s">
         <v>105</v>
@@ -2565,7 +2621,7 @@
         <v>52</v>
       </c>
       <c r="B149" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C149" t="s">
         <v>105</v>
@@ -2573,10 +2629,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B150" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C150" t="s">
         <v>105</v>
@@ -2584,10 +2640,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="B151" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C151" t="s">
         <v>105</v>
@@ -2595,10 +2651,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B152" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C152" t="s">
         <v>105</v>
@@ -2606,10 +2662,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B153" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C153" t="s">
         <v>105</v>
@@ -2617,10 +2673,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B154" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C154" t="s">
         <v>105</v>
@@ -2628,10 +2684,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
       <c r="B155" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C155" t="s">
         <v>105</v>
@@ -2639,10 +2695,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C156" t="s">
         <v>105</v>
@@ -2650,10 +2706,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="B157" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C157" t="s">
         <v>105</v>
@@ -2661,10 +2717,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
       <c r="B158" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C158" t="s">
         <v>105</v>
@@ -2672,32 +2728,32 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="B159" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C159" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B160" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C160" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B161" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
@@ -2705,10 +2761,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B162" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C162" t="s">
         <v>105</v>
@@ -2716,32 +2772,32 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B163" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C163" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B164" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C164" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B165" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C165" t="s">
         <v>107</v>
@@ -2749,10 +2805,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B166" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C166" t="s">
         <v>107</v>
@@ -2760,10 +2816,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B167" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C167" t="s">
         <v>105</v>
@@ -2771,10 +2827,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B168" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C168" t="s">
         <v>105</v>
@@ -2782,14 +2838,149 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B169" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C169" t="s">
-        <v>105</v>
-      </c>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>156</v>
+      </c>
+      <c r="B170" t="s">
+        <v>150</v>
+      </c>
+      <c r="C170" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>157</v>
+      </c>
+      <c r="B171" t="s">
+        <v>150</v>
+      </c>
+      <c r="C171" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>158</v>
+      </c>
+      <c r="B172" t="s">
+        <v>150</v>
+      </c>
+      <c r="C172" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>159</v>
+      </c>
+      <c r="B173" t="s">
+        <v>150</v>
+      </c>
+      <c r="C173" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>181</v>
+      </c>
+      <c r="B174" t="s">
+        <v>150</v>
+      </c>
+      <c r="C174" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>182</v>
+      </c>
+      <c r="B175" t="s">
+        <v>150</v>
+      </c>
+      <c r="C175" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>183</v>
+      </c>
+      <c r="B176" t="s">
+        <v>150</v>
+      </c>
+      <c r="C176" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>184</v>
+      </c>
+      <c r="B177" t="s">
+        <v>150</v>
+      </c>
+      <c r="C177" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>186</v>
+      </c>
+      <c r="B178" t="s">
+        <v>150</v>
+      </c>
+      <c r="C178" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>185</v>
+      </c>
+      <c r="B179" t="s">
+        <v>150</v>
+      </c>
+      <c r="C179" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>162</v>
+      </c>
+      <c r="B180" t="s">
+        <v>161</v>
+      </c>
+      <c r="C180" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>163</v>
+      </c>
+      <c r="B181" t="s">
+        <v>161</v>
+      </c>
+      <c r="C181" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
downloadable functionality for databse added
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_managers_report/email_alerts/www/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE20827-CF59-F94C-B1B5-0A9AF04CFA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4590F6A-9041-4642-B9AE-D8F767E89396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24400" windowHeight="13880" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="189">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -652,11 +652,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,14 +674,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -720,7 +715,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -826,7 +821,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -968,7 +963,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -976,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,7 +1172,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
@@ -1188,7 +1183,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>103</v>
@@ -1199,7 +1194,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>103</v>
@@ -1210,7 +1205,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>103</v>
@@ -1221,7 +1216,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
         <v>103</v>
@@ -1232,7 +1227,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>103</v>
@@ -1243,7 +1238,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>103</v>
@@ -1254,7 +1249,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>103</v>
@@ -1265,7 +1260,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>103</v>
@@ -1276,7 +1271,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>103</v>
@@ -1287,7 +1282,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>103</v>
@@ -1298,7 +1293,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>103</v>
@@ -1309,7 +1304,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>103</v>
@@ -1320,7 +1315,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>103</v>
@@ -1331,7 +1326,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
         <v>103</v>
@@ -1342,7 +1337,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>103</v>
@@ -1353,7 +1348,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>103</v>
@@ -1364,7 +1359,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
@@ -1375,7 +1370,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>103</v>
@@ -1386,7 +1381,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
         <v>103</v>
@@ -1397,7 +1392,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>103</v>
@@ -1408,7 +1403,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
@@ -1419,7 +1414,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>103</v>
@@ -1430,7 +1425,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>103</v>
@@ -1441,7 +1436,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>103</v>
@@ -1452,7 +1447,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>103</v>
@@ -1463,7 +1458,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>103</v>
@@ -1474,7 +1469,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
@@ -1485,7 +1480,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
         <v>103</v>
@@ -1496,7 +1491,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
@@ -1507,7 +1502,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
         <v>103</v>
@@ -1518,7 +1513,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
         <v>103</v>
@@ -1529,7 +1524,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
         <v>103</v>
@@ -1540,7 +1535,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
         <v>103</v>
@@ -1551,7 +1546,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
@@ -1562,7 +1557,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
         <v>103</v>
@@ -1573,7 +1568,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
         <v>103</v>
@@ -1584,7 +1579,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
         <v>103</v>
@@ -1595,7 +1590,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>103</v>
@@ -1606,7 +1601,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
         <v>103</v>
@@ -1617,7 +1612,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>103</v>
@@ -1628,7 +1623,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
         <v>103</v>
@@ -1639,7 +1634,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>103</v>
@@ -1650,7 +1645,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
@@ -1661,7 +1656,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -1672,7 +1667,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
         <v>103</v>
@@ -1683,7 +1678,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
         <v>103</v>
@@ -1694,7 +1689,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -1705,7 +1700,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
         <v>103</v>
@@ -1716,7 +1711,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
@@ -1727,7 +1722,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
@@ -1738,7 +1733,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
         <v>103</v>
@@ -1749,7 +1744,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
         <v>103</v>
@@ -1760,7 +1755,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>103</v>
@@ -1771,7 +1766,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
         <v>103</v>
@@ -1782,7 +1777,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
         <v>103</v>
@@ -1793,7 +1788,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
         <v>103</v>
@@ -1804,7 +1799,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="B75" t="s">
         <v>103</v>
@@ -1815,7 +1810,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
         <v>103</v>
@@ -1826,7 +1821,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
@@ -1837,7 +1832,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
         <v>103</v>
@@ -1848,7 +1843,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>103</v>
@@ -1859,7 +1854,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
         <v>103</v>
@@ -1870,7 +1865,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
         <v>103</v>
@@ -1881,7 +1876,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
@@ -1892,7 +1887,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
         <v>103</v>
@@ -1903,7 +1898,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B84" t="s">
         <v>103</v>
@@ -1914,7 +1909,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
@@ -1925,7 +1920,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B86" t="s">
         <v>103</v>
@@ -1936,7 +1931,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B87" t="s">
         <v>103</v>
@@ -1947,7 +1942,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
         <v>103</v>
@@ -1958,7 +1953,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B89" t="s">
         <v>103</v>
@@ -1969,7 +1964,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
@@ -1980,7 +1975,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
@@ -1991,29 +1986,29 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C92" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B93" t="s">
         <v>145</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="B94" t="s">
         <v>145</v>
@@ -2024,7 +2019,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
         <v>145</v>
@@ -2034,19 +2029,19 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B96" s="3" t="s">
+      <c r="A96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s">
         <v>145</v>
@@ -2057,7 +2052,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B98" t="s">
         <v>145</v>
@@ -2068,7 +2063,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s">
         <v>145</v>
@@ -2079,7 +2074,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -2090,7 +2085,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B101" t="s">
         <v>145</v>
@@ -2101,7 +2096,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
         <v>145</v>
@@ -2111,8 +2106,8 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>114</v>
+      <c r="A103" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -2122,30 +2117,30 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>179</v>
+      <c r="A104" t="s">
+        <v>178</v>
       </c>
       <c r="B104" t="s">
         <v>145</v>
       </c>
       <c r="C104" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
         <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
         <v>145</v>
@@ -2156,7 +2151,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
         <v>145</v>
@@ -2167,7 +2162,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="B108" t="s">
         <v>145</v>
@@ -2178,7 +2173,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="B109" t="s">
         <v>145</v>
@@ -2189,7 +2184,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B110" t="s">
         <v>145</v>
@@ -2200,7 +2195,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B111" t="s">
         <v>145</v>
@@ -2211,7 +2206,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B112" t="s">
         <v>145</v>
@@ -2222,7 +2217,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B113" t="s">
         <v>145</v>
@@ -2233,7 +2228,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B114" t="s">
         <v>145</v>
@@ -2244,7 +2239,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B115" t="s">
         <v>145</v>
@@ -2255,40 +2250,40 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B116" t="s">
         <v>145</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B117" t="s">
         <v>145</v>
       </c>
       <c r="C117" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B118" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C118" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B119" t="s">
         <v>144</v>
@@ -2299,7 +2294,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="B120" t="s">
         <v>144</v>
@@ -2310,7 +2305,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="B121" t="s">
         <v>144</v>
@@ -2321,7 +2316,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
@@ -2332,7 +2327,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
@@ -2343,7 +2338,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
@@ -2354,7 +2349,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -2365,7 +2360,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
         <v>144</v>
@@ -2376,7 +2371,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="B127" t="s">
         <v>144</v>
@@ -2387,7 +2382,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B128" t="s">
         <v>144</v>
@@ -2398,7 +2393,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="B129" t="s">
         <v>144</v>
@@ -2409,7 +2404,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="B130" t="s">
         <v>144</v>
@@ -2420,7 +2415,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B131" t="s">
         <v>144</v>
@@ -2431,7 +2426,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="B132" t="s">
         <v>144</v>
@@ -2442,7 +2437,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="B133" t="s">
         <v>144</v>
@@ -2453,7 +2448,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>176</v>
+        <v>34</v>
       </c>
       <c r="B134" t="s">
         <v>144</v>
@@ -2464,7 +2459,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B135" t="s">
         <v>144</v>
@@ -2475,7 +2470,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B136" t="s">
         <v>144</v>
@@ -2486,7 +2481,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B137" t="s">
         <v>144</v>
@@ -2497,9 +2492,9 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>44</v>
-      </c>
-      <c r="B138" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B138" t="s">
         <v>144</v>
       </c>
       <c r="C138" t="s">
@@ -2508,7 +2503,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B139" t="s">
         <v>144</v>
@@ -2519,7 +2514,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>49</v>
+        <v>167</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -2530,7 +2525,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B141" t="s">
         <v>144</v>
@@ -2541,7 +2536,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B142" t="s">
         <v>144</v>
@@ -2552,7 +2547,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -2563,7 +2558,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
@@ -2574,7 +2569,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="B145" t="s">
         <v>144</v>
@@ -2585,7 +2580,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B146" t="s">
         <v>144</v>
@@ -2596,7 +2591,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B147" t="s">
         <v>144</v>
@@ -2607,7 +2602,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="B148" t="s">
         <v>144</v>
@@ -2618,7 +2613,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B149" t="s">
         <v>144</v>
@@ -2629,7 +2624,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="B150" t="s">
         <v>144</v>
@@ -2640,7 +2635,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="B151" t="s">
         <v>144</v>
@@ -2651,7 +2646,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B152" t="s">
         <v>144</v>
@@ -2662,7 +2657,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="B153" t="s">
         <v>144</v>
@@ -2673,7 +2668,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B154" t="s">
         <v>144</v>
@@ -2684,7 +2679,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="B155" t="s">
         <v>144</v>
@@ -2695,7 +2690,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="B156" t="s">
         <v>144</v>
@@ -2706,7 +2701,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B157" t="s">
         <v>144</v>
@@ -2717,7 +2712,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B158" t="s">
         <v>144</v>
@@ -2728,7 +2723,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>90</v>
+        <v>168</v>
       </c>
       <c r="B159" t="s">
         <v>144</v>
@@ -2739,10 +2734,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B160" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
@@ -2750,7 +2745,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="B161" t="s">
         <v>150</v>
@@ -2761,7 +2756,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="B162" t="s">
         <v>150</v>
@@ -2772,7 +2767,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B163" t="s">
         <v>150</v>
@@ -2783,18 +2778,18 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B164" t="s">
         <v>150</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B165" t="s">
         <v>150</v>
@@ -2805,18 +2800,18 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B166" t="s">
         <v>150</v>
       </c>
       <c r="C166" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B167" t="s">
         <v>150</v>
@@ -2827,18 +2822,18 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B168" t="s">
         <v>150</v>
       </c>
       <c r="C168" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B169" t="s">
         <v>150</v>
@@ -2849,7 +2844,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B170" t="s">
         <v>150</v>
@@ -2860,7 +2855,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B171" t="s">
         <v>150</v>
@@ -2871,18 +2866,18 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B172" t="s">
         <v>150</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="B173" t="s">
         <v>150</v>
@@ -2893,7 +2888,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B174" t="s">
         <v>150</v>
@@ -2904,7 +2899,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B175" t="s">
         <v>150</v>
@@ -2915,7 +2910,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B176" t="s">
         <v>150</v>
@@ -2926,7 +2921,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B177" t="s">
         <v>150</v>
@@ -2937,7 +2932,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B178" t="s">
         <v>150</v>
@@ -2948,10 +2943,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="B179" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C179" t="s">
         <v>105</v>
@@ -2959,7 +2954,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B180" t="s">
         <v>161</v>
@@ -2969,18 +2964,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>163</v>
-      </c>
-      <c r="B181" t="s">
-        <v>161</v>
-      </c>
-      <c r="C181" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="2"/>
+      <c r="A181" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding ash and hemlock to the list
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_managers_report/email_alerts/www/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4590F6A-9041-4642-B9AE-D8F767E89396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8A428A-AC1E-3143-828C-7B5151F5E8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24400" windowHeight="13880" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="193">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -602,6 +602,18 @@
   </si>
   <si>
     <t>Vincetoxicum rossicum</t>
+  </si>
+  <si>
+    <t>Fraxinus pennsylvanica</t>
+  </si>
+  <si>
+    <t>Fraxinus americana</t>
+  </si>
+  <si>
+    <t>Fraxinus nigra</t>
+  </si>
+  <si>
+    <t>Tsuga canadensis</t>
   </si>
 </sst>
 </file>
@@ -971,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1437,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>190</v>
       </c>
       <c r="B41" t="s">
         <v>103</v>
@@ -1436,7 +1448,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
         <v>103</v>
@@ -1447,7 +1459,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="B43" t="s">
         <v>103</v>
@@ -1458,7 +1470,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
         <v>103</v>
@@ -1469,7 +1481,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
@@ -1480,7 +1492,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>103</v>
@@ -1491,7 +1503,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
@@ -1502,7 +1514,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>172</v>
       </c>
       <c r="B48" t="s">
         <v>103</v>
@@ -1513,7 +1525,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>103</v>
@@ -1524,7 +1536,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>103</v>
@@ -1535,7 +1547,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>103</v>
@@ -1546,7 +1558,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>103</v>
@@ -1557,7 +1569,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>103</v>
@@ -1568,7 +1580,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>103</v>
@@ -1579,7 +1591,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>103</v>
@@ -1590,7 +1602,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>103</v>
@@ -1601,7 +1613,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>103</v>
@@ -1612,7 +1624,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="B58" t="s">
         <v>103</v>
@@ -1623,7 +1635,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>103</v>
@@ -1634,7 +1646,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>103</v>
@@ -1645,7 +1657,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
@@ -1656,7 +1668,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -1667,7 +1679,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>103</v>
@@ -1678,7 +1690,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>103</v>
@@ -1689,7 +1701,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -1700,7 +1712,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>103</v>
@@ -1711,7 +1723,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
@@ -1722,7 +1734,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
@@ -1733,7 +1745,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>103</v>
@@ -1744,7 +1756,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>103</v>
@@ -1755,7 +1767,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>103</v>
@@ -1766,7 +1778,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>103</v>
@@ -1777,7 +1789,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>103</v>
@@ -1788,7 +1800,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>103</v>
@@ -1799,7 +1811,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>103</v>
@@ -1810,7 +1822,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
         <v>103</v>
@@ -1821,7 +1833,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
@@ -1832,7 +1844,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="B78" t="s">
         <v>103</v>
@@ -1843,7 +1855,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
         <v>103</v>
@@ -1854,7 +1866,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
         <v>103</v>
@@ -1865,7 +1877,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
         <v>103</v>
@@ -1876,7 +1888,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
@@ -1887,7 +1899,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
         <v>103</v>
@@ -1898,7 +1910,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
         <v>103</v>
@@ -1909,7 +1921,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
@@ -1920,7 +1932,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
         <v>103</v>
@@ -1931,7 +1943,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="B87" t="s">
         <v>103</v>
@@ -1942,7 +1954,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B88" t="s">
         <v>103</v>
@@ -1953,7 +1965,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
         <v>103</v>
@@ -1964,7 +1976,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
@@ -1975,7 +1987,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
@@ -1986,62 +1998,62 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B96" t="s">
         <v>145</v>
       </c>
       <c r="C96" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B97" t="s">
         <v>145</v>
@@ -2052,7 +2064,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>187</v>
       </c>
       <c r="B98" t="s">
         <v>145</v>
@@ -2063,7 +2075,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s">
         <v>145</v>
@@ -2074,7 +2086,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -2085,7 +2097,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B101" t="s">
         <v>145</v>
@@ -2096,7 +2108,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B102" t="s">
         <v>145</v>
@@ -2106,8 +2118,8 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>179</v>
+      <c r="A103" t="s">
+        <v>111</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -2118,18 +2130,18 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="B104" t="s">
         <v>145</v>
       </c>
       <c r="C104" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="B105" t="s">
         <v>145</v>
@@ -2140,7 +2152,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B106" t="s">
         <v>145</v>
@@ -2150,8 +2162,8 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>175</v>
+      <c r="A107" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B107" t="s">
         <v>145</v>
@@ -2162,18 +2174,18 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="B108" t="s">
         <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="B109" t="s">
         <v>145</v>
@@ -2184,7 +2196,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B110" t="s">
         <v>145</v>
@@ -2195,7 +2207,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="B111" t="s">
         <v>145</v>
@@ -2206,7 +2218,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="B112" t="s">
         <v>145</v>
@@ -2217,7 +2229,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B113" t="s">
         <v>145</v>
@@ -2228,7 +2240,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B114" t="s">
         <v>145</v>
@@ -2239,7 +2251,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B115" t="s">
         <v>145</v>
@@ -2250,18 +2262,18 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B116" t="s">
         <v>145</v>
       </c>
       <c r="C116" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B117" t="s">
         <v>145</v>
@@ -2272,32 +2284,32 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C118" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B119" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C119" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C120" t="s">
         <v>105</v>
@@ -2305,18 +2317,18 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B121" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
@@ -2327,7 +2339,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
@@ -2338,7 +2350,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
@@ -2349,7 +2361,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -2360,7 +2372,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="B126" t="s">
         <v>144</v>
@@ -2371,7 +2383,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
         <v>144</v>
@@ -2382,7 +2394,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="B128" t="s">
         <v>144</v>
@@ -2393,7 +2405,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="B129" t="s">
         <v>144</v>
@@ -2404,7 +2416,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>17</v>
       </c>
       <c r="B130" t="s">
         <v>144</v>
@@ -2415,7 +2427,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B131" t="s">
         <v>144</v>
@@ -2426,7 +2438,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B132" t="s">
         <v>144</v>
@@ -2437,7 +2449,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="B133" t="s">
         <v>144</v>
@@ -2448,7 +2460,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="B134" t="s">
         <v>144</v>
@@ -2459,7 +2471,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="B135" t="s">
         <v>144</v>
@@ -2470,7 +2482,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B136" t="s">
         <v>144</v>
@@ -2481,7 +2493,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="B137" t="s">
         <v>144</v>
@@ -2492,7 +2504,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B138" t="s">
         <v>144</v>
@@ -2503,7 +2515,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B139" t="s">
         <v>144</v>
@@ -2514,7 +2526,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -2525,7 +2537,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="B141" t="s">
         <v>144</v>
@@ -2536,7 +2548,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="B142" t="s">
         <v>144</v>
@@ -2547,7 +2559,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -2558,7 +2570,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
@@ -2569,7 +2581,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B145" t="s">
         <v>144</v>
@@ -2580,7 +2592,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B146" t="s">
         <v>144</v>
@@ -2591,7 +2603,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="B147" t="s">
         <v>144</v>
@@ -2602,7 +2614,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B148" t="s">
         <v>144</v>
@@ -2613,7 +2625,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B149" t="s">
         <v>144</v>
@@ -2624,7 +2636,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="B150" t="s">
         <v>144</v>
@@ -2635,7 +2647,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B151" t="s">
         <v>144</v>
@@ -2646,7 +2658,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
       <c r="B152" t="s">
         <v>144</v>
@@ -2657,7 +2669,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B153" t="s">
         <v>144</v>
@@ -2668,7 +2680,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B154" t="s">
         <v>144</v>
@@ -2679,7 +2691,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B155" t="s">
         <v>144</v>
@@ -2690,7 +2702,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="B156" t="s">
         <v>144</v>
@@ -2701,7 +2713,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B157" t="s">
         <v>144</v>
@@ -2712,7 +2724,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B158" t="s">
         <v>144</v>
@@ -2723,7 +2735,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="B159" t="s">
         <v>144</v>
@@ -2734,10 +2746,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B160" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
@@ -2745,10 +2757,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>180</v>
+        <v>87</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
@@ -2756,10 +2768,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="B162" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C162" t="s">
         <v>105</v>
@@ -2767,10 +2779,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B163" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C163" t="s">
         <v>105</v>
@@ -2778,29 +2790,29 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B164" t="s">
         <v>150</v>
       </c>
       <c r="C164" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="B165" t="s">
         <v>150</v>
       </c>
       <c r="C165" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B166" t="s">
         <v>150</v>
@@ -2811,7 +2823,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B167" t="s">
         <v>150</v>
@@ -2822,7 +2834,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B168" t="s">
         <v>150</v>
@@ -2833,7 +2845,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B169" t="s">
         <v>150</v>
@@ -2844,73 +2856,73 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B170" t="s">
         <v>150</v>
       </c>
       <c r="C170" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B171" t="s">
         <v>150</v>
       </c>
       <c r="C171" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B172" t="s">
         <v>150</v>
       </c>
       <c r="C172" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="B173" t="s">
         <v>150</v>
       </c>
       <c r="C173" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="B174" t="s">
         <v>150</v>
       </c>
       <c r="C174" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B175" t="s">
         <v>150</v>
       </c>
       <c r="C175" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B176" t="s">
         <v>150</v>
@@ -2921,7 +2933,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B177" t="s">
         <v>150</v>
@@ -2932,7 +2944,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B178" t="s">
         <v>150</v>
@@ -2943,10 +2955,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="B179" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C179" t="s">
         <v>105</v>
@@ -2954,17 +2966,61 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>184</v>
+      </c>
+      <c r="B180" t="s">
+        <v>150</v>
+      </c>
+      <c r="C180" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>186</v>
+      </c>
+      <c r="B181" t="s">
+        <v>150</v>
+      </c>
+      <c r="C181" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>185</v>
+      </c>
+      <c r="B182" t="s">
+        <v>150</v>
+      </c>
+      <c r="C182" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>162</v>
+      </c>
+      <c r="B183" t="s">
+        <v>161</v>
+      </c>
+      <c r="C183" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>163</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B184" t="s">
         <v>161</v>
       </c>
-      <c r="C180" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="2"/>
+      <c r="C184" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding black bear and changing to all obs not just RG
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_managers_report/email_alerts/www/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8A428A-AC1E-3143-828C-7B5151F5E8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D317D7F2-BDDF-104B-B168-86ECD469F895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="194">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>Tsuga canadensis</t>
+  </si>
+  <si>
+    <t>Ursus americanus</t>
   </si>
 </sst>
 </file>
@@ -983,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1965,7 +1968,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
         <v>103</v>
@@ -1976,7 +1979,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
@@ -1987,7 +1990,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
@@ -1998,7 +2001,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
         <v>103</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
         <v>103</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
         <v>103</v>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
         <v>103</v>
@@ -2042,29 +2045,29 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
         <v>145</v>
       </c>
       <c r="C97" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="B98" t="s">
         <v>145</v>
@@ -2075,7 +2078,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
         <v>145</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -2097,7 +2100,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
         <v>145</v>
@@ -2108,7 +2111,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
         <v>145</v>
@@ -2119,7 +2122,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -2130,7 +2133,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s">
         <v>145</v>
@@ -2141,7 +2144,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" t="s">
         <v>145</v>
@@ -2152,7 +2155,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
         <v>145</v>
@@ -2162,8 +2165,8 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>179</v>
+      <c r="A107" t="s">
+        <v>114</v>
       </c>
       <c r="B107" t="s">
         <v>145</v>
@@ -2173,30 +2176,30 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>178</v>
+      <c r="A108" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B108" t="s">
         <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B109" t="s">
         <v>145</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="B110" t="s">
         <v>145</v>
@@ -2207,7 +2210,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B111" t="s">
         <v>145</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
         <v>145</v>
@@ -2229,7 +2232,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="B113" t="s">
         <v>145</v>
@@ -2240,7 +2243,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
         <v>145</v>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
         <v>145</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
         <v>145</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
         <v>145</v>
@@ -2284,7 +2287,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
         <v>145</v>
@@ -2295,7 +2298,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
         <v>145</v>
@@ -2306,40 +2309,40 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
         <v>145</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
         <v>145</v>
       </c>
       <c r="C121" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C122" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
         <v>144</v>
@@ -2383,7 +2386,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="B127" t="s">
         <v>144</v>
@@ -2394,7 +2397,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B128" t="s">
         <v>144</v>
@@ -2405,7 +2408,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="B129" t="s">
         <v>144</v>
@@ -2416,7 +2419,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="B130" t="s">
         <v>144</v>
@@ -2427,7 +2430,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="B131" t="s">
         <v>144</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B132" t="s">
         <v>144</v>
@@ -2449,7 +2452,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="B133" t="s">
         <v>144</v>
@@ -2460,7 +2463,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="B134" t="s">
         <v>144</v>
@@ -2471,7 +2474,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
         <v>144</v>
@@ -2482,7 +2485,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
         <v>144</v>
@@ -2493,7 +2496,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>176</v>
+        <v>32</v>
       </c>
       <c r="B137" t="s">
         <v>144</v>
@@ -2504,7 +2507,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
         <v>144</v>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B139" t="s">
         <v>144</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -2537,7 +2540,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B141" t="s">
         <v>144</v>
@@ -2548,7 +2551,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B142" t="s">
         <v>144</v>
@@ -2559,7 +2562,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -2570,7 +2573,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>49</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
@@ -2581,7 +2584,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="B145" t="s">
         <v>144</v>
@@ -2592,7 +2595,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B146" t="s">
         <v>144</v>
@@ -2603,7 +2606,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="B147" t="s">
         <v>144</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B148" t="s">
         <v>144</v>
@@ -2625,7 +2628,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B149" t="s">
         <v>144</v>
@@ -2636,7 +2639,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B150" t="s">
         <v>144</v>
@@ -2647,7 +2650,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B151" t="s">
         <v>144</v>
@@ -2658,7 +2661,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B152" t="s">
         <v>144</v>
@@ -2669,7 +2672,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B153" t="s">
         <v>144</v>
@@ -2680,7 +2683,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="B154" t="s">
         <v>144</v>
@@ -2691,7 +2694,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="B155" t="s">
         <v>144</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
         <v>144</v>
@@ -2713,7 +2716,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="B157" t="s">
         <v>144</v>
@@ -2724,7 +2727,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B158" t="s">
         <v>144</v>
@@ -2735,7 +2738,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="B159" t="s">
         <v>144</v>
@@ -2746,7 +2749,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="B160" t="s">
         <v>144</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B161" t="s">
         <v>144</v>
@@ -2768,7 +2771,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B162" t="s">
         <v>144</v>
@@ -2779,7 +2782,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="B163" t="s">
         <v>144</v>
@@ -2790,10 +2793,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B164" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C164" t="s">
         <v>105</v>
@@ -2801,7 +2804,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="B165" t="s">
         <v>150</v>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
         <v>150</v>
@@ -2823,7 +2826,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B167" t="s">
         <v>150</v>
@@ -2834,18 +2837,18 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B168" t="s">
         <v>150</v>
       </c>
       <c r="C168" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B169" t="s">
         <v>150</v>
@@ -2856,18 +2859,18 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B170" t="s">
         <v>150</v>
       </c>
       <c r="C170" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B171" t="s">
         <v>150</v>
@@ -2878,18 +2881,18 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B172" t="s">
         <v>150</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B173" t="s">
         <v>150</v>
@@ -2900,7 +2903,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B174" t="s">
         <v>150</v>
@@ -2911,7 +2914,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B175" t="s">
         <v>150</v>
@@ -2922,18 +2925,18 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B176" t="s">
         <v>150</v>
       </c>
       <c r="C176" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B177" t="s">
         <v>150</v>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178" t="s">
         <v>150</v>
@@ -2955,7 +2958,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B179" t="s">
         <v>150</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B180" t="s">
         <v>150</v>
@@ -2977,7 +2980,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B181" t="s">
         <v>150</v>
@@ -2988,7 +2991,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B182" t="s">
         <v>150</v>
@@ -2999,10 +3002,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C183" t="s">
         <v>105</v>
@@ -3010,7 +3013,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B184" t="s">
         <v>161</v>
@@ -3020,7 +3023,18 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="2"/>
+      <c r="A185" t="s">
+        <v>163</v>
+      </c>
+      <c r="B185" t="s">
+        <v>161</v>
+      </c>
+      <c r="C185" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding black bear and allowing non-RG obs
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_managers_report/email_alerts/www/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8A428A-AC1E-3143-828C-7B5151F5E8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8395357-1427-4C46-B754-85F0D56DD89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="194">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>Tsuga canadensis</t>
+  </si>
+  <si>
+    <t>Ursus americanus</t>
   </si>
 </sst>
 </file>
@@ -983,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="118" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1965,7 +1968,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
         <v>103</v>
@@ -1976,7 +1979,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
@@ -1987,7 +1990,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
@@ -1998,7 +2001,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
         <v>103</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
         <v>103</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
         <v>103</v>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
         <v>103</v>
@@ -2042,29 +2045,29 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
         <v>145</v>
       </c>
       <c r="C97" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="B98" t="s">
         <v>145</v>
@@ -2075,7 +2078,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
         <v>145</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -2097,7 +2100,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
         <v>145</v>
@@ -2108,7 +2111,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
         <v>145</v>
@@ -2119,7 +2122,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -2130,7 +2133,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s">
         <v>145</v>
@@ -2141,7 +2144,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" t="s">
         <v>145</v>
@@ -2152,7 +2155,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
         <v>145</v>
@@ -2162,8 +2165,8 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>179</v>
+      <c r="A107" t="s">
+        <v>114</v>
       </c>
       <c r="B107" t="s">
         <v>145</v>
@@ -2173,30 +2176,30 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>178</v>
+      <c r="A108" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B108" t="s">
         <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B109" t="s">
         <v>145</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="B110" t="s">
         <v>145</v>
@@ -2207,7 +2210,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B111" t="s">
         <v>145</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
         <v>145</v>
@@ -2229,7 +2232,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="B113" t="s">
         <v>145</v>
@@ -2240,7 +2243,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
         <v>145</v>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
         <v>145</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
         <v>145</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
         <v>145</v>
@@ -2284,7 +2287,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
         <v>145</v>
@@ -2295,7 +2298,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
         <v>145</v>
@@ -2306,40 +2309,40 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
         <v>145</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
         <v>145</v>
       </c>
       <c r="C121" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C122" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123" t="s">
         <v>144</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
         <v>144</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="B125" t="s">
         <v>144</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
         <v>144</v>
@@ -2383,7 +2386,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="B127" t="s">
         <v>144</v>
@@ -2394,7 +2397,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B128" t="s">
         <v>144</v>
@@ -2405,7 +2408,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="B129" t="s">
         <v>144</v>
@@ -2416,7 +2419,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="B130" t="s">
         <v>144</v>
@@ -2427,7 +2430,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="B131" t="s">
         <v>144</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B132" t="s">
         <v>144</v>
@@ -2449,7 +2452,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="B133" t="s">
         <v>144</v>
@@ -2460,7 +2463,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="B134" t="s">
         <v>144</v>
@@ -2471,7 +2474,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
         <v>144</v>
@@ -2482,7 +2485,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
         <v>144</v>
@@ -2493,7 +2496,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>176</v>
+        <v>32</v>
       </c>
       <c r="B137" t="s">
         <v>144</v>
@@ -2504,7 +2507,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
         <v>144</v>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B139" t="s">
         <v>144</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -2537,7 +2540,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B141" t="s">
         <v>144</v>
@@ -2548,7 +2551,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B142" t="s">
         <v>144</v>
@@ -2559,7 +2562,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B143" t="s">
         <v>144</v>
@@ -2570,7 +2573,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>49</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
@@ -2581,7 +2584,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="B145" t="s">
         <v>144</v>
@@ -2592,7 +2595,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B146" t="s">
         <v>144</v>
@@ -2603,7 +2606,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="B147" t="s">
         <v>144</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B148" t="s">
         <v>144</v>
@@ -2625,7 +2628,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="B149" t="s">
         <v>144</v>
@@ -2636,7 +2639,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B150" t="s">
         <v>144</v>
@@ -2647,7 +2650,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B151" t="s">
         <v>144</v>
@@ -2658,7 +2661,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B152" t="s">
         <v>144</v>
@@ -2669,7 +2672,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B153" t="s">
         <v>144</v>
@@ -2680,7 +2683,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="B154" t="s">
         <v>144</v>
@@ -2691,7 +2694,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="B155" t="s">
         <v>144</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
         <v>144</v>
@@ -2713,7 +2716,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="B157" t="s">
         <v>144</v>
@@ -2724,7 +2727,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B158" t="s">
         <v>144</v>
@@ -2735,7 +2738,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="B159" t="s">
         <v>144</v>
@@ -2746,7 +2749,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="B160" t="s">
         <v>144</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B161" t="s">
         <v>144</v>
@@ -2768,7 +2771,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B162" t="s">
         <v>144</v>
@@ -2779,7 +2782,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="B163" t="s">
         <v>144</v>
@@ -2790,10 +2793,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B164" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C164" t="s">
         <v>105</v>
@@ -2801,7 +2804,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="B165" t="s">
         <v>150</v>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
         <v>150</v>
@@ -2823,7 +2826,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B167" t="s">
         <v>150</v>
@@ -2834,18 +2837,18 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B168" t="s">
         <v>150</v>
       </c>
       <c r="C168" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B169" t="s">
         <v>150</v>
@@ -2856,18 +2859,18 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B170" t="s">
         <v>150</v>
       </c>
       <c r="C170" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B171" t="s">
         <v>150</v>
@@ -2878,18 +2881,18 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B172" t="s">
         <v>150</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B173" t="s">
         <v>150</v>
@@ -2900,7 +2903,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B174" t="s">
         <v>150</v>
@@ -2911,7 +2914,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B175" t="s">
         <v>150</v>
@@ -2922,18 +2925,18 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B176" t="s">
         <v>150</v>
       </c>
       <c r="C176" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B177" t="s">
         <v>150</v>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178" t="s">
         <v>150</v>
@@ -2955,7 +2958,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B179" t="s">
         <v>150</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B180" t="s">
         <v>150</v>
@@ -2977,7 +2980,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B181" t="s">
         <v>150</v>
@@ -2988,7 +2991,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B182" t="s">
         <v>150</v>
@@ -2999,10 +3002,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C183" t="s">
         <v>105</v>
@@ -3010,7 +3013,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B184" t="s">
         <v>161</v>
@@ -3020,7 +3023,18 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="2"/>
+      <c r="A185" t="s">
+        <v>163</v>
+      </c>
+      <c r="B185" t="s">
+        <v>161</v>
+      </c>
+      <c r="C185" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding buffer description and fraxinus genus
</commit_message>
<xml_diff>
--- a/email_alerts/www/datasets/acad_watchlist_species.xlsx
+++ b/email_alerts/www/datasets/acad_watchlist_species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_managers_report/email_alerts/www/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178F942-B59C-A347-A9FF-99E2015DD6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A13EB6A-24E4-214A-B376-D94556BE4626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="197">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -623,6 +623,9 @@
   </si>
   <si>
     <t>Lonicera morrowii</t>
+  </si>
+  <si>
+    <t>Fraxinus</t>
   </si>
 </sst>
 </file>
@@ -992,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="118" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2491,7 +2494,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>39</v>
+        <v>196</v>
       </c>
       <c r="B136" t="s">
         <v>103</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B137" t="s">
         <v>103</v>
@@ -2513,7 +2516,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B138" t="s">
         <v>103</v>
@@ -2524,7 +2527,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B139" t="s">
         <v>103</v>
@@ -2535,7 +2538,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B140" t="s">
         <v>103</v>
@@ -2546,7 +2549,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B141" t="s">
         <v>103</v>
@@ -2557,7 +2560,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B142" t="s">
         <v>103</v>
@@ -2568,7 +2571,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B143" t="s">
         <v>103</v>
@@ -2579,7 +2582,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B144" t="s">
         <v>103</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B145" t="s">
         <v>103</v>
@@ -2601,7 +2604,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B146" t="s">
         <v>103</v>
@@ -2612,7 +2615,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B147" t="s">
         <v>103</v>
@@ -2623,7 +2626,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="B148" t="s">
         <v>103</v>
@@ -2634,7 +2637,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="B149" t="s">
         <v>103</v>
@@ -2645,7 +2648,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>160</v>
+        <v>57</v>
       </c>
       <c r="B150" t="s">
         <v>103</v>
@@ -2656,7 +2659,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="B151" t="s">
         <v>103</v>
@@ -2667,7 +2670,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B152" t="s">
         <v>103</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B153" t="s">
         <v>103</v>
@@ -2689,7 +2692,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B154" t="s">
         <v>103</v>
@@ -2700,7 +2703,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B155" t="s">
         <v>103</v>
@@ -2711,7 +2714,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B156" t="s">
         <v>103</v>
@@ -2722,7 +2725,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B157" t="s">
         <v>103</v>
@@ -2733,7 +2736,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B158" t="s">
         <v>103</v>
@@ -2744,7 +2747,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B159" t="s">
         <v>103</v>
@@ -2755,7 +2758,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B160" t="s">
         <v>103</v>
@@ -2766,7 +2769,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B161" t="s">
         <v>103</v>
@@ -2777,7 +2780,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B162" t="s">
         <v>103</v>
@@ -2788,7 +2791,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B163" t="s">
         <v>103</v>
@@ -2799,7 +2802,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B164" t="s">
         <v>103</v>
@@ -2810,7 +2813,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B165" t="s">
         <v>103</v>
@@ -2821,7 +2824,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B166" t="s">
         <v>103</v>
@@ -2832,7 +2835,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B167" t="s">
         <v>103</v>
@@ -2843,7 +2846,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B168" t="s">
         <v>103</v>
@@ -2854,7 +2857,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B169" t="s">
         <v>103</v>
@@ -2865,7 +2868,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B170" t="s">
         <v>103</v>
@@ -2876,7 +2879,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B171" t="s">
         <v>103</v>
@@ -2887,7 +2890,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B172" t="s">
         <v>103</v>
@@ -2898,7 +2901,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B173" t="s">
         <v>103</v>
@@ -2909,7 +2912,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B174" t="s">
         <v>103</v>
@@ -2920,7 +2923,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B175" t="s">
         <v>103</v>
@@ -2931,7 +2934,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B176" t="s">
         <v>103</v>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B177" t="s">
         <v>103</v>
@@ -2953,7 +2956,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>192</v>
+        <v>89</v>
       </c>
       <c r="B178" t="s">
         <v>103</v>
@@ -2964,7 +2967,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="B179" t="s">
         <v>103</v>
@@ -2975,7 +2978,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
       <c r="B180" t="s">
         <v>103</v>
@@ -2986,7 +2989,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="B181" t="s">
         <v>103</v>
@@ -2997,7 +3000,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B182" t="s">
         <v>103</v>
@@ -3008,7 +3011,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B183" t="s">
         <v>103</v>
@@ -3019,7 +3022,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B184" t="s">
         <v>103</v>
@@ -3030,7 +3033,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B185" t="s">
         <v>103</v>
@@ -3041,7 +3044,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B186" t="s">
         <v>103</v>
@@ -3052,22 +3055,33 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>96</v>
+      </c>
+      <c r="B187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C187" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
         <v>97</v>
       </c>
-      <c r="B187" t="s">
-        <v>103</v>
-      </c>
-      <c r="C187" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="2"/>
+      <c r="B188" t="s">
+        <v>103</v>
+      </c>
+      <c r="C188" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C188">
-    <sortCondition ref="B2:B188"/>
-    <sortCondition ref="A2:A188"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C189">
+    <sortCondition ref="B2:B189"/>
+    <sortCondition ref="A2:A189"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>